<commit_message>
Association of footprints. Add footprints, one left. Add datasheets. Update BOM
</commit_message>
<xml_diff>
--- a/EEG_v2_BOM.xlsx
+++ b/EEG_v2_BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="180">
   <si>
     <t>ref</t>
   </si>
@@ -318,9 +318,6 @@
     <t>X1</t>
   </si>
   <si>
-    <t>32-KHz</t>
-  </si>
-  <si>
     <t>~</t>
   </si>
   <si>
@@ -526,6 +523,42 @@
   </si>
   <si>
     <t>Footprints to do</t>
+  </si>
+  <si>
+    <t>CRCW08051M00FKEA</t>
+  </si>
+  <si>
+    <t>LM2664M6X/NOPB</t>
+  </si>
+  <si>
+    <t>TI</t>
+  </si>
+  <si>
+    <t>CC2540F256RHAR</t>
+  </si>
+  <si>
+    <t>TLV70033DDCR</t>
+  </si>
+  <si>
+    <t>TLV70025DDCR</t>
+  </si>
+  <si>
+    <t>TPS72325DBVR</t>
+  </si>
+  <si>
+    <t>0805</t>
+  </si>
+  <si>
+    <t>0603</t>
+  </si>
+  <si>
+    <t>0402</t>
+  </si>
+  <si>
+    <t>32.768-KHz</t>
+  </si>
+  <si>
+    <t>ssss810701</t>
   </si>
 </sst>
 </file>
@@ -1009,7 +1042,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1022,6 +1055,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1346,8 +1385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:K57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O37" sqref="O37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1362,22 +1401,22 @@
   <sheetData>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
         <v>104</v>
       </c>
-      <c r="D4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>105</v>
-      </c>
-      <c r="F4" t="s">
-        <v>106</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>2</v>
@@ -1385,7 +1424,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>23</v>
@@ -1397,21 +1436,21 @@
         <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F5" t="s">
-        <v>117</v>
-      </c>
-      <c r="G5" t="s">
+        <v>116</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -1420,21 +1459,21 @@
         <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F6" t="s">
-        <v>125</v>
-      </c>
-      <c r="G6" t="s">
+        <v>124</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -1443,21 +1482,21 @@
         <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F7" t="s">
-        <v>126</v>
-      </c>
-      <c r="G7" t="s">
+        <v>125</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -1466,18 +1505,18 @@
         <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F8" t="s">
-        <v>127</v>
-      </c>
-      <c r="G8" t="s">
+        <v>126</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>27</v>
@@ -1489,18 +1528,18 @@
         <v>29</v>
       </c>
       <c r="E9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F9" t="s">
-        <v>128</v>
-      </c>
-      <c r="G9" t="s">
+        <v>127</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>8</v>
@@ -1512,21 +1551,21 @@
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F10" t="s">
-        <v>146</v>
-      </c>
-      <c r="G10">
-        <v>805</v>
+        <v>145</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C11">
         <v>17</v>
@@ -1535,18 +1574,18 @@
         <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F11" t="s">
-        <v>129</v>
-      </c>
-      <c r="G11" t="s">
+        <v>128</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>17</v>
@@ -1558,21 +1597,21 @@
         <v>18</v>
       </c>
       <c r="E12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F12" t="s">
-        <v>147</v>
-      </c>
-      <c r="G12">
-        <v>805</v>
+        <v>146</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C13">
         <v>5</v>
@@ -1581,21 +1620,21 @@
         <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F13" t="s">
-        <v>130</v>
-      </c>
-      <c r="G13" t="s">
+        <v>129</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C14">
         <v>9</v>
@@ -1604,21 +1643,21 @@
         <v>20</v>
       </c>
       <c r="E14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F14" t="s">
-        <v>131</v>
-      </c>
-      <c r="G14" t="s">
+        <v>130</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C15">
         <v>12</v>
@@ -1627,21 +1666,21 @@
         <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F15" t="s">
-        <v>132</v>
-      </c>
-      <c r="G15" t="s">
+        <v>131</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -1650,21 +1689,21 @@
         <v>5</v>
       </c>
       <c r="E16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F16" t="s">
-        <v>148</v>
-      </c>
-      <c r="G16">
-        <v>805</v>
+        <v>147</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C17">
         <v>2</v>
@@ -1673,18 +1712,18 @@
         <v>16</v>
       </c>
       <c r="E17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F17" t="s">
-        <v>149</v>
-      </c>
-      <c r="G17">
-        <v>805</v>
+        <v>148</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>13</v>
@@ -1696,18 +1735,18 @@
         <v>14</v>
       </c>
       <c r="E18" t="s">
+        <v>139</v>
+      </c>
+      <c r="F18" t="s">
         <v>140</v>
       </c>
-      <c r="F18" t="s">
-        <v>141</v>
-      </c>
-      <c r="G18" t="s">
+      <c r="G18" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>10</v>
@@ -1719,18 +1758,18 @@
         <v>11</v>
       </c>
       <c r="E19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F19" t="s">
-        <v>142</v>
-      </c>
-      <c r="G19" t="s">
+        <v>141</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>30</v>
@@ -1742,18 +1781,18 @@
         <v>31</v>
       </c>
       <c r="E20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F20" t="s">
-        <v>143</v>
-      </c>
-      <c r="G20">
-        <v>603</v>
+        <v>142</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>32</v>
@@ -1765,13 +1804,13 @@
         <v>33</v>
       </c>
       <c r="E21" t="s">
+        <v>143</v>
+      </c>
+      <c r="F21" t="s">
         <v>144</v>
       </c>
-      <c r="F21" t="s">
-        <v>145</v>
-      </c>
-      <c r="G21">
-        <v>603</v>
+      <c r="G21" s="6" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1784,13 +1823,13 @@
       <c r="D22" t="s">
         <v>35</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>37</v>
@@ -1802,13 +1841,13 @@
         <v>38</v>
       </c>
       <c r="E23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F23" t="s">
-        <v>134</v>
-      </c>
-      <c r="G23">
-        <v>402</v>
+        <v>133</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -1821,7 +1860,7 @@
       <c r="D24" t="s">
         <v>40</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="5" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1835,13 +1874,13 @@
       <c r="D25" t="s">
         <v>50</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25" s="5" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>43</v>
@@ -1853,12 +1892,12 @@
         <v>44</v>
       </c>
       <c r="E26" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F26" t="s">
         <v>45</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G26" s="5" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1872,13 +1911,13 @@
       <c r="D27" t="s">
         <v>47</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G27" s="5" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C28">
         <v>2</v>
@@ -1886,16 +1925,16 @@
       <c r="D28" t="s">
         <v>41</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G28" s="5" t="s">
         <v>42</v>
       </c>
       <c r="K28" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>57</v>
@@ -1907,16 +1946,16 @@
         <v>0</v>
       </c>
       <c r="E29" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F29" t="s">
-        <v>150</v>
-      </c>
-      <c r="G29">
+        <v>149</v>
+      </c>
+      <c r="G29" s="5">
         <v>402</v>
       </c>
       <c r="J29" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K29" t="s">
         <v>36</v>
@@ -1924,10 +1963,10 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C30">
         <v>2</v>
@@ -1936,16 +1975,16 @@
         <v>33</v>
       </c>
       <c r="E30" t="s">
+        <v>150</v>
+      </c>
+      <c r="F30" t="s">
         <v>151</v>
       </c>
-      <c r="F30" t="s">
-        <v>152</v>
-      </c>
-      <c r="G30" t="s">
+      <c r="G30" s="5" t="s">
         <v>61</v>
       </c>
       <c r="J30" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K30" t="s">
         <v>42</v>
@@ -1953,10 +1992,10 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C31">
         <v>2</v>
@@ -1965,16 +2004,16 @@
         <v>270</v>
       </c>
       <c r="E31" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F31" t="s">
-        <v>153</v>
-      </c>
-      <c r="G31" t="s">
+        <v>152</v>
+      </c>
+      <c r="G31" s="5" t="s">
         <v>60</v>
       </c>
       <c r="J31" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K31" t="s">
         <v>51</v>
@@ -1982,7 +2021,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>62</v>
@@ -1994,16 +2033,16 @@
         <v>63</v>
       </c>
       <c r="E32" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F32" t="s">
-        <v>154</v>
-      </c>
-      <c r="G32" t="s">
+        <v>153</v>
+      </c>
+      <c r="G32" s="5" t="s">
         <v>61</v>
       </c>
       <c r="J32" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K32" t="s">
         <v>48</v>
@@ -2011,10 +2050,10 @@
     </row>
     <row r="33" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C33">
         <v>18</v>
@@ -2023,16 +2062,16 @@
         <v>54</v>
       </c>
       <c r="E33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F33" t="s">
-        <v>155</v>
-      </c>
-      <c r="G33">
-        <v>603</v>
+        <v>154</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>176</v>
       </c>
       <c r="J33" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K33" t="s">
         <v>45</v>
@@ -2040,7 +2079,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>52</v>
@@ -2052,24 +2091,24 @@
         <v>53</v>
       </c>
       <c r="E34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F34" t="s">
-        <v>158</v>
-      </c>
-      <c r="G34">
-        <v>603</v>
+        <v>157</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>176</v>
       </c>
       <c r="J34" t="s">
+        <v>162</v>
+      </c>
+      <c r="K34" t="s">
         <v>163</v>
-      </c>
-      <c r="K34" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>58</v>
@@ -2081,13 +2120,16 @@
         <v>59</v>
       </c>
       <c r="E35" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F35" t="s">
-        <v>157</v>
-      </c>
-      <c r="G35" t="s">
+        <v>156</v>
+      </c>
+      <c r="G35" s="5" t="s">
         <v>60</v>
+      </c>
+      <c r="J35" t="s">
+        <v>162</v>
       </c>
       <c r="K35" t="s">
         <v>95</v>
@@ -2095,7 +2137,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>55</v>
@@ -2106,16 +2148,22 @@
       <c r="D36" t="s">
         <v>56</v>
       </c>
-      <c r="G36">
-        <v>805</v>
+      <c r="E36" t="s">
+        <v>155</v>
+      </c>
+      <c r="F36" t="s">
+        <v>168</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>175</v>
       </c>
       <c r="K36" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>64</v>
@@ -2127,16 +2175,19 @@
         <v>65</v>
       </c>
       <c r="E37" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F37" t="s">
         <v>66</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G37" s="5" t="s">
         <v>66</v>
       </c>
+      <c r="J37" t="s">
+        <v>162</v>
+      </c>
       <c r="K37" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -2150,24 +2201,27 @@
         <v>68</v>
       </c>
       <c r="E38" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F38" t="s">
-        <v>135</v>
-      </c>
-      <c r="G38" t="s">
+        <v>134</v>
+      </c>
+      <c r="G38" s="5" t="s">
         <v>69</v>
       </c>
+      <c r="J38" t="s">
+        <v>162</v>
+      </c>
       <c r="K38" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C39">
         <v>2</v>
@@ -2176,13 +2230,19 @@
         <v>70</v>
       </c>
       <c r="E39" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F39" t="s">
-        <v>135</v>
-      </c>
-      <c r="G39" t="s">
+        <v>134</v>
+      </c>
+      <c r="G39" s="5" t="s">
         <v>69</v>
+      </c>
+      <c r="J39" t="s">
+        <v>162</v>
+      </c>
+      <c r="K39" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -2196,9 +2256,9 @@
         <v>75</v>
       </c>
       <c r="F40" t="s">
-        <v>138</v>
-      </c>
-      <c r="G40" t="s">
+        <v>137</v>
+      </c>
+      <c r="G40" s="5" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2213,9 +2273,9 @@
         <v>72</v>
       </c>
       <c r="F41" t="s">
-        <v>138</v>
-      </c>
-      <c r="G41" t="s">
+        <v>137</v>
+      </c>
+      <c r="G41" s="5" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2230,9 +2290,9 @@
         <v>77</v>
       </c>
       <c r="F42" t="s">
-        <v>138</v>
-      </c>
-      <c r="G42" t="s">
+        <v>137</v>
+      </c>
+      <c r="G42" s="5" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2247,15 +2307,15 @@
         <v>79</v>
       </c>
       <c r="F43" t="s">
-        <v>138</v>
-      </c>
-      <c r="G43" t="s">
+        <v>137</v>
+      </c>
+      <c r="G43" s="5" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>96</v>
@@ -2267,18 +2327,18 @@
         <v>97</v>
       </c>
       <c r="E44" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F44" t="s">
         <v>97</v>
       </c>
-      <c r="G44" t="s">
+      <c r="G44" s="5" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>88</v>
@@ -2289,13 +2349,19 @@
       <c r="D45" t="s">
         <v>89</v>
       </c>
-      <c r="G45" t="s">
+      <c r="E45" t="s">
+        <v>170</v>
+      </c>
+      <c r="F45" t="s">
+        <v>169</v>
+      </c>
+      <c r="G45" s="5" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>80</v>
@@ -2306,13 +2372,19 @@
       <c r="D46" t="s">
         <v>81</v>
       </c>
-      <c r="G46" t="s">
+      <c r="E46" t="s">
+        <v>170</v>
+      </c>
+      <c r="F46" t="s">
+        <v>81</v>
+      </c>
+      <c r="G46" s="5" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>83</v>
@@ -2323,13 +2395,19 @@
       <c r="D47" t="s">
         <v>84</v>
       </c>
-      <c r="G47" t="s">
+      <c r="E47" t="s">
+        <v>170</v>
+      </c>
+      <c r="F47" t="s">
+        <v>172</v>
+      </c>
+      <c r="G47" s="5" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>86</v>
@@ -2340,13 +2418,19 @@
       <c r="D48" t="s">
         <v>87</v>
       </c>
-      <c r="G48" t="s">
+      <c r="E48" t="s">
+        <v>170</v>
+      </c>
+      <c r="F48" t="s">
+        <v>173</v>
+      </c>
+      <c r="G48" s="5" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>91</v>
@@ -2357,13 +2441,19 @@
       <c r="D49" t="s">
         <v>92</v>
       </c>
-      <c r="G49" t="s">
+      <c r="E49" t="s">
+        <v>170</v>
+      </c>
+      <c r="F49" t="s">
+        <v>174</v>
+      </c>
+      <c r="G49" s="5" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>93</v>
@@ -2374,36 +2464,42 @@
       <c r="D50" t="s">
         <v>94</v>
       </c>
-      <c r="G50" t="s">
+      <c r="E50" t="s">
+        <v>170</v>
+      </c>
+      <c r="F50" t="s">
+        <v>171</v>
+      </c>
+      <c r="G50" s="5" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B51" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51" t="s">
         <v>101</v>
       </c>
-      <c r="C51">
-        <v>1</v>
-      </c>
-      <c r="D51" t="s">
+      <c r="E51" t="s">
+        <v>159</v>
+      </c>
+      <c r="F51" t="s">
+        <v>158</v>
+      </c>
+      <c r="G51" s="5" t="s">
         <v>102</v>
-      </c>
-      <c r="E51" t="s">
-        <v>160</v>
-      </c>
-      <c r="F51" t="s">
-        <v>159</v>
-      </c>
-      <c r="G51" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>98</v>
@@ -2412,16 +2508,16 @@
         <v>1</v>
       </c>
       <c r="D52" t="s">
+        <v>178</v>
+      </c>
+      <c r="E52" t="s">
+        <v>159</v>
+      </c>
+      <c r="F52" t="s">
+        <v>160</v>
+      </c>
+      <c r="G52" s="5" t="s">
         <v>99</v>
-      </c>
-      <c r="E52" t="s">
-        <v>160</v>
-      </c>
-      <c r="F52" t="s">
-        <v>161</v>
-      </c>
-      <c r="G52" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Continue layout, test antenna workings
</commit_message>
<xml_diff>
--- a/EEG_v2_BOM.xlsx
+++ b/EEG_v2_BOM.xlsx
@@ -1042,7 +1042,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1061,6 +1061,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1386,7 +1389,7 @@
   <dimension ref="A4:K57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O37" sqref="O37"/>
+      <selection activeCell="B9" sqref="B5:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1426,7 +1429,7 @@
       <c r="A5" t="s">
         <v>161</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="7" t="s">
         <v>23</v>
       </c>
       <c r="C5">
@@ -1449,7 +1452,7 @@
       <c r="A6" t="s">
         <v>161</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="7" t="s">
         <v>118</v>
       </c>
       <c r="C6">
@@ -1472,7 +1475,7 @@
       <c r="A7" t="s">
         <v>161</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="7" t="s">
         <v>119</v>
       </c>
       <c r="C7">
@@ -1495,7 +1498,7 @@
       <c r="A8" t="s">
         <v>161</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="7" t="s">
         <v>120</v>
       </c>
       <c r="C8">
@@ -1518,7 +1521,7 @@
       <c r="A9" t="s">
         <v>161</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="7" t="s">
         <v>27</v>
       </c>
       <c r="C9">
@@ -1564,7 +1567,7 @@
       <c r="A11" t="s">
         <v>161</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="7" t="s">
         <v>106</v>
       </c>
       <c r="C11">
@@ -1610,7 +1613,7 @@
       <c r="A13" t="s">
         <v>161</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="7" t="s">
         <v>107</v>
       </c>
       <c r="C13">
@@ -1633,7 +1636,7 @@
       <c r="A14" t="s">
         <v>161</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="7" t="s">
         <v>121</v>
       </c>
       <c r="C14">
@@ -1656,7 +1659,7 @@
       <c r="A15" t="s">
         <v>161</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="7" t="s">
         <v>108</v>
       </c>
       <c r="C15">

</xml_diff>